<commit_message>
naplóóraszámok valós és leadott frissítve
</commit_message>
<xml_diff>
--- a/naplooraszamok.xlsx
+++ b/naplooraszamok.xlsx
@@ -15,6 +15,9 @@
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <customWorkbookViews>
+    <customWorkbookView name="Nova - Egyéni nézet" guid="{8E69CA9E-D7E8-4B96-A536-5F888A6AB13A}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
+  </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="14">
   <si>
     <t>mocsi</t>
   </si>
@@ -64,6 +67,9 @@
   <si>
     <t>leadott</t>
   </si>
+  <si>
+    <t>Össz SZUM</t>
+  </si>
 </sst>
 </file>
 
@@ -92,7 +98,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -119,6 +125,48 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -165,7 +213,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -197,13 +245,25 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="2" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Jó" xfId="1" builtinId="26"/>
@@ -220,6 +280,70 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{A7F80C7F-3D2E-40AA-AF9A-F55F5A713CE4}" diskRevisions="1" revisionId="2" version="2">
+  <header guid="{F81EC625-5E7F-4BBB-92DB-8137AB7E486B}" dateTime="2018-05-14T02:48:21" maxSheetId="2" userName="Nova" r:id="rId1">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{A7F80C7F-3D2E-40AA-AF9A-F55F5A713CE4}" dateTime="2018-05-14T02:50:07" maxSheetId="2" userName="Nova" r:id="rId2" minRId="1" maxRId="2">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+</headers>
+</file>
+
+<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
+</file>
+
+<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="H30">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="O30">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rcc rId="1" sId="1">
+    <oc r="L17">
+      <v>0</v>
+    </oc>
+    <nc r="L17">
+      <v>5</v>
+    </nc>
+  </rcc>
+  <rcc rId="2" sId="1">
+    <oc r="M17">
+      <v>0</v>
+    </oc>
+    <nc r="M17">
+      <v>5</v>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
+  <userInfo guid="{A7F80C7F-3D2E-40AA-AF9A-F55F5A713CE4}" name="Nova" id="-892390432" dateTime="2018-05-14T02:48:21"/>
+</users>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -485,15 +609,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:O34"/>
+  <dimension ref="A2:R35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
@@ -863,45 +987,45 @@
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C11" s="18">
+      <c r="C11" s="17">
         <f>C10/SUM($C$10:$G$10)</f>
         <v>0.28871391076115488</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="17">
         <f>D10/SUM($C$10:$G$10)</f>
         <v>0.28608923884514437</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E11" s="17">
         <f>E10/SUM($C$10:$G$10)</f>
         <v>0.13123359580052493</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F11" s="17">
         <f>F10/SUM($C$10:$G$10)</f>
         <v>0.14173228346456693</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G11" s="17">
         <f>G10/SUM($C$10:$G$10)</f>
         <v>0.15223097112860892</v>
       </c>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18">
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17">
         <f>J10/SUM($J$10:$N$10)</f>
         <v>0.30054644808743169</v>
       </c>
-      <c r="K11" s="18">
+      <c r="K11" s="17">
         <f>K10/SUM($J$10:$N$10)</f>
         <v>0.29781420765027322</v>
       </c>
-      <c r="L11" s="18">
+      <c r="L11" s="17">
         <f>L10/SUM($J$10:$N$10)</f>
         <v>9.5628415300546443E-2</v>
       </c>
-      <c r="M11" s="18">
+      <c r="M11" s="17">
         <f>M10/SUM($J$10:$N$10)</f>
         <v>0.14754098360655737</v>
       </c>
-      <c r="N11" s="18">
+      <c r="N11" s="17">
         <f>N10/SUM($J$10:$N$10)</f>
         <v>0.15846994535519127</v>
       </c>
@@ -1024,7 +1148,7 @@
       </c>
       <c r="O16" s="7"/>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B17" s="5">
         <v>8</v>
       </c>
@@ -1035,10 +1159,10 @@
         <v>23.5</v>
       </c>
       <c r="E17" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F17" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G17" s="5">
         <v>0</v>
@@ -1052,17 +1176,17 @@
         <v>23.5</v>
       </c>
       <c r="L17" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M17" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N17" s="5">
         <v>0</v>
       </c>
       <c r="O17" s="7"/>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B18" s="5">
         <v>9</v>
       </c>
@@ -1100,7 +1224,7 @@
       </c>
       <c r="O18" s="7"/>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
         <v>5</v>
       </c>
@@ -1114,11 +1238,11 @@
       </c>
       <c r="E19" s="6">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F19" s="6">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G19" s="6">
         <f t="shared" si="4"/>
@@ -1126,7 +1250,7 @@
       </c>
       <c r="H19" s="13">
         <f>SUM(C19:G19)</f>
-        <v>58.5</v>
+        <v>68.5</v>
       </c>
       <c r="I19" s="13" t="s">
         <v>5</v>
@@ -1141,11 +1265,11 @@
       </c>
       <c r="L19" s="6">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="M19" s="6">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="N19" s="6">
         <f t="shared" si="5"/>
@@ -1153,66 +1277,66 @@
       </c>
       <c r="O19" s="8">
         <f>SUM(J19:N19)</f>
-        <v>58.5</v>
-      </c>
-    </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+        <v>68.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
-      <c r="C20" s="18">
+      <c r="C20" s="17">
         <f>C19/SUM($C$19:$G$19)</f>
-        <v>0.31623931623931623</v>
-      </c>
-      <c r="D20" s="18">
+        <v>0.27007299270072993</v>
+      </c>
+      <c r="D20" s="17">
         <f>D19/SUM($C$19:$G$19)</f>
-        <v>0.49572649572649574</v>
-      </c>
-      <c r="E20" s="18">
+        <v>0.42335766423357662</v>
+      </c>
+      <c r="E20" s="17">
         <f>E19/SUM($C$19:$G$19)</f>
-        <v>1.7094017094017096E-2</v>
-      </c>
-      <c r="F20" s="18">
+        <v>8.7591240875912413E-2</v>
+      </c>
+      <c r="F20" s="17">
         <f>F19/SUM($C$19:$G$19)</f>
-        <v>0.10256410256410256</v>
-      </c>
-      <c r="G20" s="18">
+        <v>0.16058394160583941</v>
+      </c>
+      <c r="G20" s="17">
         <f>G19/SUM($C$19:$G$19)</f>
-        <v>6.8376068376068383E-2</v>
-      </c>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18">
+        <v>5.8394160583941604E-2</v>
+      </c>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17">
         <f>J19/SUM($J$19:$N$19)</f>
-        <v>0.31623931623931623</v>
-      </c>
-      <c r="K20" s="18">
+        <v>0.27007299270072993</v>
+      </c>
+      <c r="K20" s="17">
         <f>K19/SUM($J$19:$N$19)</f>
-        <v>0.49572649572649574</v>
-      </c>
-      <c r="L20" s="18">
+        <v>0.42335766423357662</v>
+      </c>
+      <c r="L20" s="17">
         <f>L19/SUM($J$19:$N$19)</f>
-        <v>1.7094017094017096E-2</v>
-      </c>
-      <c r="M20" s="18">
+        <v>8.7591240875912413E-2</v>
+      </c>
+      <c r="M20" s="17">
         <f>M19/SUM($J$19:$N$19)</f>
-        <v>0.10256410256410256</v>
-      </c>
-      <c r="N20" s="18">
+        <v>0.16058394160583941</v>
+      </c>
+      <c r="N20" s="17">
         <f>N19/SUM($J$19:$N$19)</f>
-        <v>6.8376068376068383E-2</v>
+        <v>5.8394160583941604E-2</v>
       </c>
       <c r="O20" s="7"/>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
       <c r="O21" s="7"/>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
       <c r="O22" s="7"/>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>9</v>
       </c>
@@ -1230,7 +1354,7 @@
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
@@ -1250,7 +1374,7 @@
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
         <v>0</v>
@@ -1286,255 +1410,358 @@
       </c>
       <c r="O25" s="7"/>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B26" s="4">
         <v>10</v>
       </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
+      <c r="C26" s="4">
+        <v>10</v>
+      </c>
+      <c r="D26" s="4">
+        <v>16</v>
+      </c>
+      <c r="E26" s="4">
+        <v>10</v>
+      </c>
+      <c r="F26" s="4">
+        <v>8</v>
+      </c>
+      <c r="G26" s="4">
+        <v>8.5</v>
+      </c>
       <c r="H26" s="9"/>
       <c r="I26" s="10"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
+      <c r="J26" s="4">
+        <v>10</v>
+      </c>
+      <c r="K26" s="4">
+        <v>16</v>
+      </c>
+      <c r="L26" s="4">
+        <v>10</v>
+      </c>
+      <c r="M26" s="4">
+        <v>8</v>
+      </c>
+      <c r="N26" s="4">
+        <v>8.5</v>
+      </c>
       <c r="O26" s="7"/>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B27" s="5">
         <v>11</v>
       </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
+      <c r="C27" s="5">
+        <v>10</v>
+      </c>
+      <c r="D27" s="5">
+        <v>11</v>
+      </c>
+      <c r="E27" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="F27" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="G27" s="5">
+        <v>3.5</v>
+      </c>
       <c r="H27" s="11"/>
       <c r="I27" s="12"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="5"/>
-      <c r="M27" s="5"/>
-      <c r="N27" s="5"/>
+      <c r="J27" s="5">
+        <v>10</v>
+      </c>
+      <c r="K27" s="5">
+        <v>11</v>
+      </c>
+      <c r="L27" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="M27" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="N27" s="5">
+        <v>3.5</v>
+      </c>
       <c r="O27" s="7"/>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B28" s="6">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="1">
+        <f>SUM(C26:C27)</f>
+        <v>20</v>
+      </c>
+      <c r="D28" s="1">
+        <f>SUM(D26:D27)</f>
+        <v>27</v>
+      </c>
+      <c r="E28" s="1">
+        <f>SUM(E26:E27)</f>
+        <v>11.5</v>
+      </c>
+      <c r="F28" s="1">
+        <f>SUM(F26:F27)</f>
+        <v>10.5</v>
+      </c>
+      <c r="G28" s="1">
+        <f>SUM(G26:G27)</f>
         <v>12</v>
       </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
-      <c r="L28" s="6"/>
-      <c r="M28" s="6"/>
-      <c r="N28" s="6"/>
-      <c r="O28" s="7"/>
-    </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B29" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" s="1">
-        <f>SUM(C26:C28)</f>
-        <v>0</v>
-      </c>
-      <c r="D29" s="1">
-        <f t="shared" ref="D29" si="6">SUM(D26:D28)</f>
-        <v>0</v>
-      </c>
-      <c r="E29" s="1">
-        <f t="shared" ref="E29" si="7">SUM(E26:E28)</f>
-        <v>0</v>
-      </c>
-      <c r="F29" s="1">
-        <f t="shared" ref="F29" si="8">SUM(F26:F28)</f>
-        <v>0</v>
-      </c>
-      <c r="G29" s="1">
-        <f t="shared" ref="G29" si="9">SUM(G26:G28)</f>
-        <v>0</v>
-      </c>
-      <c r="H29" s="16">
-        <f>SUM(C29:G29)</f>
-        <v>0</v>
-      </c>
-      <c r="I29" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="J29" s="1">
-        <f>SUM(J26:J28)</f>
-        <v>0</v>
-      </c>
-      <c r="K29" s="1">
-        <f t="shared" ref="K29" si="10">SUM(K26:K28)</f>
-        <v>0</v>
-      </c>
-      <c r="L29" s="1">
-        <f t="shared" ref="L29" si="11">SUM(L26:L28)</f>
-        <v>0</v>
-      </c>
-      <c r="M29" s="1">
-        <f t="shared" ref="M29" si="12">SUM(M26:M28)</f>
-        <v>0</v>
-      </c>
-      <c r="N29" s="1">
-        <f t="shared" ref="N29" si="13">SUM(N26:N28)</f>
-        <v>0</v>
-      </c>
-      <c r="O29" s="8">
-        <f>SUM(J29:N29)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="18">
-        <f>C29/SUM($C$19:$G$19)</f>
-        <v>0</v>
-      </c>
-      <c r="D30" s="18">
-        <f>D29/SUM($C$19:$G$19)</f>
-        <v>0</v>
-      </c>
-      <c r="E30" s="18">
-        <v>0.2</v>
-      </c>
-      <c r="F30" s="18">
-        <f>F29/SUM($C$19:$G$19)</f>
-        <v>0</v>
-      </c>
-      <c r="G30" s="18">
-        <f>G29/SUM($C$19:$G$19)</f>
-        <v>0</v>
-      </c>
-      <c r="H30" s="19"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="18">
-        <f>J29/SUM($J$19:$N$19)</f>
-        <v>0</v>
-      </c>
-      <c r="K30" s="18">
-        <f>K29/SUM($J$19:$N$19)</f>
-        <v>0</v>
-      </c>
-      <c r="L30" s="18">
-        <f>L29/SUM($J$19:$N$19)</f>
-        <v>0</v>
-      </c>
-      <c r="M30" s="18">
-        <f>M29/SUM($J$19:$N$19)</f>
-        <v>0</v>
-      </c>
-      <c r="N30" s="18">
-        <f>N29/SUM($J$19:$N$19)</f>
-        <v>0</v>
-      </c>
-      <c r="O30" s="7"/>
-    </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
+      <c r="H28" s="15">
+        <f>SUM(C28:G28)</f>
+        <v>81</v>
+      </c>
+      <c r="I28" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="J28" s="1">
+        <f>SUM(J26:J27)</f>
+        <v>20</v>
+      </c>
+      <c r="K28" s="1">
+        <f>SUM(K26:K27)</f>
+        <v>27</v>
+      </c>
+      <c r="L28" s="1">
+        <f>SUM(L26:L27)</f>
+        <v>11.5</v>
+      </c>
+      <c r="M28" s="1">
+        <f>SUM(M26:M27)</f>
+        <v>10.5</v>
+      </c>
+      <c r="N28" s="1">
+        <f>SUM(N26:N27)</f>
+        <v>12</v>
+      </c>
+      <c r="O28" s="8">
+        <f>SUM(J28:N28)</f>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B29" s="1"/>
+      <c r="C29" s="17">
+        <f>C28/SUM($C$28:$G$28)</f>
+        <v>0.24691358024691357</v>
+      </c>
+      <c r="D29" s="17">
+        <f t="shared" ref="D29:G29" si="6">D28/SUM($C$28:$G$28)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E29" s="17">
+        <f t="shared" si="6"/>
+        <v>0.1419753086419753</v>
+      </c>
+      <c r="F29" s="17">
+        <f t="shared" si="6"/>
+        <v>0.12962962962962962</v>
+      </c>
+      <c r="G29" s="17">
+        <f t="shared" si="6"/>
+        <v>0.14814814814814814</v>
+      </c>
+      <c r="H29" s="18"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="17">
+        <f>J28/SUM($J$28:$N$28)</f>
+        <v>0.24691358024691357</v>
+      </c>
+      <c r="K29" s="17">
+        <f t="shared" ref="K29:N29" si="7">K28/SUM($J$28:$N$28)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="L29" s="17">
+        <f t="shared" si="7"/>
+        <v>0.1419753086419753</v>
+      </c>
+      <c r="M29" s="17">
+        <f t="shared" si="7"/>
+        <v>0.12962962962962962</v>
+      </c>
+      <c r="N29" s="17">
+        <f t="shared" si="7"/>
+        <v>0.14814814814814814</v>
+      </c>
+      <c r="O29" s="7"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" s="19"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="22"/>
+      <c r="J30" s="21"/>
+      <c r="K30" s="21"/>
+      <c r="L30" s="21"/>
+      <c r="M30" s="21"/>
+      <c r="N30" s="21"/>
+      <c r="O30" s="19"/>
+      <c r="P30" s="19"/>
+      <c r="Q30" s="19"/>
+      <c r="R30" s="19"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B31" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="26">
+        <f>C28+C19+C10</f>
+        <v>93.5</v>
+      </c>
+      <c r="D31" s="26">
+        <f t="shared" ref="D31:G31" si="8">D28+D19+D10</f>
+        <v>110.5</v>
+      </c>
+      <c r="E31" s="26">
+        <f t="shared" si="8"/>
+        <v>42.5</v>
+      </c>
+      <c r="F31" s="26">
+        <f t="shared" si="8"/>
+        <v>48.5</v>
+      </c>
+      <c r="G31" s="26">
+        <f t="shared" si="8"/>
+        <v>45</v>
+      </c>
+      <c r="H31" s="23">
+        <f>H10+H19+H28</f>
+        <v>340</v>
+      </c>
+      <c r="J31" s="26">
+        <f>J28+J19+J10</f>
+        <v>93.5</v>
+      </c>
+      <c r="K31" s="26">
+        <f t="shared" ref="K31:N31" si="9">K28+K19+K10</f>
+        <v>110.5</v>
+      </c>
+      <c r="L31" s="26">
+        <f t="shared" si="9"/>
+        <v>35</v>
+      </c>
+      <c r="M31" s="26">
+        <f t="shared" si="9"/>
+        <v>48.5</v>
+      </c>
+      <c r="N31" s="26">
+        <f t="shared" si="9"/>
+        <v>45</v>
+      </c>
+      <c r="O31" s="23">
+        <f>O10+O19+O28</f>
+        <v>332.5</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B33" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C32">
+      <c r="C33" s="25">
         <f>(C19+C10)/(SUM($C10:$G10)+SUM($C19:$G19))</f>
-        <v>0.29518072289156627</v>
-      </c>
-      <c r="D32">
+        <v>0.28378378378378377</v>
+      </c>
+      <c r="D33" s="25">
         <f>(D19+D10)/(SUM($C10:$G10)+SUM($C19:$G19))</f>
-        <v>0.3353413654618474</v>
-      </c>
-      <c r="E32">
-        <f t="shared" ref="E32:G32" si="14">(E19+E10)/(SUM($C10:$G10)+SUM($C19:$G19))</f>
-        <v>0.10441767068273092</v>
-      </c>
-      <c r="F32">
-        <f t="shared" si="14"/>
-        <v>0.13253012048192772</v>
-      </c>
-      <c r="G32">
-        <f t="shared" si="14"/>
-        <v>0.13253012048192772</v>
-      </c>
-      <c r="J32">
+        <v>0.32239382239382242</v>
+      </c>
+      <c r="E33" s="25">
+        <f>(E19+E10)/(SUM($C10:$G10)+SUM($C19:$G19))</f>
+        <v>0.11969111969111969</v>
+      </c>
+      <c r="F33" s="25">
+        <f>(F19+F10)/(SUM($C10:$G10)+SUM($C19:$G19))</f>
+        <v>0.14671814671814673</v>
+      </c>
+      <c r="G33" s="25">
+        <f>(G19+G10)/(SUM($C10:$G10)+SUM($C19:$G19))</f>
+        <v>0.12741312741312741</v>
+      </c>
+      <c r="J33" s="25">
         <f>(J19+J10)/(SUM($J10:$N10)+SUM($J19:$N19))</f>
-        <v>0.30434782608695654</v>
-      </c>
-      <c r="K32">
-        <f t="shared" ref="K32:N32" si="15">(K19+K10)/(SUM($J10:$N10)+SUM($J19:$N19))</f>
-        <v>0.34575569358178054</v>
-      </c>
-      <c r="L32">
-        <f t="shared" si="15"/>
-        <v>7.6604554865424432E-2</v>
-      </c>
-      <c r="M32">
-        <f t="shared" si="15"/>
-        <v>0.13664596273291926</v>
-      </c>
-      <c r="N32">
-        <f t="shared" si="15"/>
-        <v>0.13664596273291926</v>
-      </c>
-    </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+        <v>0.2922465208747515</v>
+      </c>
+      <c r="K33" s="25">
+        <f>(K19+K10)/(SUM($J10:$N10)+SUM($J19:$N19))</f>
+        <v>0.33200795228628233</v>
+      </c>
+      <c r="L33" s="25">
+        <f>(L19+L10)/(SUM($J10:$N10)+SUM($J19:$N19))</f>
+        <v>9.3439363817097415E-2</v>
+      </c>
+      <c r="M33" s="25">
+        <f>(M19+M10)/(SUM($J10:$N10)+SUM($J19:$N19))</f>
+        <v>0.15109343936381708</v>
+      </c>
+      <c r="N33" s="25">
+        <f>(N19+N10)/(SUM($J10:$N10)+SUM($J19:$N19))</f>
+        <v>0.1312127236580517</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B35" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C34" s="17">
-        <f>0.2*C11+0.5*C20+0.3*C30</f>
-        <v>0.21586244027188908</v>
-      </c>
-      <c r="D34" s="17">
-        <f>0.2*D11+0.5*D20+0.3*D30</f>
-        <v>0.30508109563227676</v>
-      </c>
-      <c r="E34" s="17">
-        <f>0.2*E11+0.5*E20+0.3*E30</f>
-        <v>9.4793727707113529E-2</v>
-      </c>
-      <c r="F34" s="17">
-        <f>0.2*F11+0.5*F20+0.3*F30</f>
-        <v>7.9628507974964666E-2</v>
-      </c>
-      <c r="G34" s="17">
-        <f>0.2*G11+0.5*G20+0.3*G30</f>
-        <v>6.4634228413755976E-2</v>
-      </c>
-      <c r="H34" s="17"/>
-      <c r="I34" s="17"/>
-      <c r="J34" s="17">
-        <f>0.2*J11+0.5*J20+0.3*J30</f>
-        <v>0.21822894773714446</v>
-      </c>
-      <c r="K34" s="17">
-        <f>0.2*K11+0.5*K20+0.3*K30</f>
-        <v>0.30742608939330252</v>
-      </c>
-      <c r="L34" s="17">
-        <f>0.2*L11+0.5*L20+0.3*L30</f>
-        <v>2.7672691607117838E-2</v>
-      </c>
-      <c r="M34" s="17">
-        <f>0.2*M11+0.5*M20+0.3*M30</f>
-        <v>8.0790248003362763E-2</v>
-      </c>
-      <c r="N34" s="17">
-        <f>0.2*N11+0.5*N20+0.3*N30</f>
-        <v>6.5882023259072442E-2</v>
+      <c r="C35" s="28">
+        <f>0.2*C11+0.5*C20+0.3*C29</f>
+        <v>0.26685335257666998</v>
+      </c>
+      <c r="D35" s="28">
+        <f>0.2*D11+0.5*D20+0.3*D29</f>
+        <v>0.36889667988581715</v>
+      </c>
+      <c r="E35" s="28">
+        <f>0.2*E11+0.5*E20+0.3*E29</f>
+        <v>0.11263493219065379</v>
+      </c>
+      <c r="F35" s="28">
+        <f>0.2*F11+0.5*F20+0.3*F29</f>
+        <v>0.14752731638472197</v>
+      </c>
+      <c r="G35" s="28">
+        <f>0.2*G11+0.5*G20+0.3*G29</f>
+        <v>0.10408771896213703</v>
+      </c>
+      <c r="H35" s="16"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="28">
+        <f>0.2*J11+0.5*J20+0.3*J29</f>
+        <v>0.26921986004192539</v>
+      </c>
+      <c r="K35" s="28">
+        <f>0.2*K11+0.5*K20+0.3*K29</f>
+        <v>0.37124167364684291</v>
+      </c>
+      <c r="L35" s="28">
+        <f>0.2*L11+0.5*L20+0.3*L29</f>
+        <v>0.10551389609065809</v>
+      </c>
+      <c r="M35" s="28">
+        <f>0.2*M11+0.5*M20+0.3*M29</f>
+        <v>0.14868905641312008</v>
+      </c>
+      <c r="N35" s="28">
+        <f>0.2*N11+0.5*N20+0.3*N29</f>
+        <v>0.1053355138074535</v>
       </c>
     </row>
   </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{8E69CA9E-D7E8-4B96-A536-5F888A6AB13A}">
+      <selection activeCell="Z28" sqref="Z28"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" r:id="rId1"/>
+    </customSheetView>
+  </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>